<commit_message>
Generate output files and plots
</commit_message>
<xml_diff>
--- a/model/UnmetDemand/Output Files/Output_1_16.xlsx
+++ b/model/UnmetDemand/Output Files/Output_1_16.xlsx
@@ -501,13 +501,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>389307.4937815363</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>389307.4937815362</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>389307.4937815362</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -605,13 +605,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>365997.894915453</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>364565.0620511367</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>363130.2854596089</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -709,13 +709,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-10397.43020010318</v>
+        <v>-33627.6</v>
       </c>
       <c r="C6" t="n">
-        <v>-8964.597335786941</v>
+        <v>-33627.6</v>
       </c>
       <c r="D6" t="n">
-        <v>-7529.820744259083</v>
+        <v>-33627.6</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -4523,37 +4523,37 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>56.31823077048233</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>221.6398701147446</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>324.61</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>322.6079999999999</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>306.592</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>304.876</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>297.4399999999964</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>272.844</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>271.414</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>214.7763725738737</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>30.62984974540833</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
         <v>0</v>
@@ -4602,34 +4602,34 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>63.17234471337443</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>228.8</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>271.7</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>271.7</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>257.4</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>257.4</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>251.68</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>228.8</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>228.8</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>112.492107257715</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -4681,34 +4681,34 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>116.4604256857013</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>263.9206921964125</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>333.19</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>333.762</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>319.748</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>320.3200000000001</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>315.172</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>292.864</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>176.432120767841</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>34.0349779106982</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
@@ -4760,37 +4760,37 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>56.31823077048233</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>221.6398701147446</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>324.61</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>322.6079999999999</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>306.592</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>304.876</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>297.4399999999962</v>
+        <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>272.844</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>271.414</v>
+        <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>214.7763725738737</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>30.62984974540832</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
         <v>0</v>
@@ -4839,34 +4839,34 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>63.17234471337443</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>228.8</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>271.7</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>271.7</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>257.4</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>257.4</v>
+        <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>251.68</v>
+        <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>228.8</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>228.8</v>
+        <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>112.492107257715</v>
+        <v>0</v>
       </c>
       <c r="S6" t="n">
         <v>0</v>
@@ -4918,34 +4918,34 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>116.4604256857013</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>263.9206921964125</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>333.19</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>333.762</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>319.748</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>320.3200000000001</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>315.172</v>
+        <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>292.864</v>
+        <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>176.432120767841</v>
+        <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>34.0349779106982</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
         <v>0</v>
@@ -4997,37 +4997,37 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>56.31823077048233</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>221.6398701147446</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>324.61</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>322.6079999999999</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>306.592</v>
+        <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>304.8759999999965</v>
+        <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>297.44</v>
+        <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>272.844</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>271.414</v>
+        <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>214.7763725738737</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>30.62984974540832</v>
+        <v>0</v>
       </c>
       <c r="T8" t="n">
         <v>0</v>
@@ -5076,34 +5076,34 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>63.17234471337443</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>228.8</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>271.7</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>271.7</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>257.4</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>257.4</v>
+        <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>251.68</v>
+        <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>228.8</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>228.8</v>
+        <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>112.492107257715</v>
+        <v>0</v>
       </c>
       <c r="S9" t="n">
         <v>0</v>
@@ -5155,34 +5155,34 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>116.4604256857013</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>263.9206921964125</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>333.19</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>333.762</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>319.748</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>320.3200000000001</v>
+        <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>315.172</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>292.864</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>176.432120767841</v>
+        <v>0</v>
       </c>
       <c r="R10" t="n">
-        <v>34.0349779106982</v>
+        <v>0</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -8150,76 +8150,76 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-370.4143528989813</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>-349.8745169153619</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-323.2990290295856</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-306.4445982054113</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>-304.2291681757649</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>-318.074690831447</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>-337.378924150804</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>-276.848</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>-283.426</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>-324.61</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>-322.6079999999999</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>-306.592</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>-304.876</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>-297.44</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>-272.844</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>-271.414</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>-261.404</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>-254.254</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>-391.5955291070197</v>
+        <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>-444.3122552611476</v>
+        <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>-436.0135784144501</v>
+        <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>-425.3355231041314</v>
+        <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>-374.0444019949066</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>-335.7333614715552</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -8229,76 +8229,76 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-288.5780292354309</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>-269.4605762365213</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>-251.562220653923</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>-236.2645485692544</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>-234.8803273813275</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>-245.8072043092885</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>-273.42333901413</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>-220.22</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>-228.8</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>-271.7</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>-271.7</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>-257.4</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>-257.4</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>-251.68</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>-228.8</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>-228.8</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>-220.22</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>-217.7131985152447</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>-326.4262376682347</v>
+        <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>-356.0438733264622</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>-353.8915634556467</v>
+        <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>-346.0470726979044</v>
+        <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>-302.770231542496</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="n">
-        <v>-283.0975195669943</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -8308,76 +8308,76 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-330.8657055718805</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>-312.5986355576808</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>-302.5194122782605</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>-287.6344989330975</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>-285.9374865868901</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>-293.0534320728443</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>-297.2998549933121</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>-280.566</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>-289.718</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>-333.19</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>-333.762</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>-319.748</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>-320.3200000000001</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>-315.172</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>-292.864</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>-293.436</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>-285.428</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>-307.9904506607303</v>
+        <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>-354.873879232159</v>
+        <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>-369.6570220893018</v>
+        <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>-374.4435484968433</v>
+        <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>-368.5746222916773</v>
+        <v>0</v>
       </c>
       <c r="X4" t="n">
-        <v>-332.7400610900855</v>
+        <v>0</v>
       </c>
       <c r="Y4" t="n">
-        <v>-331.1336776624333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -8387,76 +8387,76 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-370.4143528989813</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>-349.8745169153619</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>-323.2990290295856</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>-306.4445982054113</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>-304.2291681757649</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>-318.074690831447</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>-337.378924150804</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>-276.848</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>-283.426</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>-324.61</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>-322.6079999999999</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>-306.592</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>-304.876</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>-297.44</v>
+        <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>-272.844</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>-271.414</v>
+        <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>-261.404</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>-254.254</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>-391.5955291070197</v>
+        <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>-444.3122552611476</v>
+        <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>-436.0135784144501</v>
+        <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>-425.3355231041314</v>
+        <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>-374.0444019949066</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="n">
-        <v>-335.7333614715552</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -8466,76 +8466,76 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-288.5780292354309</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>-269.4605762365213</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>-251.562220653923</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>-236.2645485692544</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>-234.8803273813275</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>-245.8072043092885</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>-273.42333901413</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>-220.22</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>-228.8</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>-271.7</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>-271.7</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>-257.4</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>-257.4</v>
+        <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>-251.68</v>
+        <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>-228.8</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>-228.8</v>
+        <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>-220.22</v>
+        <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>-217.7131985152447</v>
+        <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>-326.4262376682347</v>
+        <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>-356.0438733264622</v>
+        <v>0</v>
       </c>
       <c r="V6" t="n">
-        <v>-353.8915634556467</v>
+        <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>-346.0470726979044</v>
+        <v>0</v>
       </c>
       <c r="X6" t="n">
-        <v>-302.770231542496</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="n">
-        <v>-283.0975195669943</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -8545,76 +8545,76 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-330.8657055718805</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>-312.5986355576808</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>-302.5194122782605</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>-287.6344989330975</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>-285.9374865868901</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>-293.0534320728443</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>-297.2998549933121</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>-280.566</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>-289.718</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>-333.19</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>-333.762</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>-319.748</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>-320.3200000000001</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>-315.172</v>
+        <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>-292.864</v>
+        <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>-293.436</v>
+        <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>-285.428</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>-307.9904506607303</v>
+        <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>-354.873879232159</v>
+        <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>-369.6570220893018</v>
+        <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>-374.4435484968433</v>
+        <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>-368.5746222916773</v>
+        <v>0</v>
       </c>
       <c r="X7" t="n">
-        <v>-332.7400610900855</v>
+        <v>0</v>
       </c>
       <c r="Y7" t="n">
-        <v>-331.1336776624333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -8624,76 +8624,76 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-370.4143528989813</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>-349.8745169153619</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>-323.2990290295856</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>-306.4445982054113</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>-304.2291681757649</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>-318.074690831447</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>-337.378924150804</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>-276.848</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>-283.426</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>-324.61</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>-322.6079999999999</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>-306.592</v>
+        <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>-304.876</v>
+        <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>-297.44</v>
+        <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>-272.844</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>-271.414</v>
+        <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>-261.404</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>-254.254</v>
+        <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>-391.5955291070197</v>
+        <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>-444.3122552611476</v>
+        <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>-436.0135784144501</v>
+        <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>-425.3355231041314</v>
+        <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>-374.0444019949066</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="n">
-        <v>-335.7333614715552</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -8703,76 +8703,76 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-288.5780292354309</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>-269.4605762365213</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>-251.562220653923</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>-236.2645485692544</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>-234.8803273813275</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>-245.8072043092885</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>-273.42333901413</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>-220.22</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>-228.8</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>-271.7</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>-271.7</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>-257.4</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>-257.4</v>
+        <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>-251.68</v>
+        <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>-228.8</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>-228.8</v>
+        <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>-220.22</v>
+        <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>-217.7131985152447</v>
+        <v>0</v>
       </c>
       <c r="T9" t="n">
-        <v>-326.4262376682347</v>
+        <v>0</v>
       </c>
       <c r="U9" t="n">
-        <v>-356.0438733264622</v>
+        <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>-353.8915634556467</v>
+        <v>0</v>
       </c>
       <c r="W9" t="n">
-        <v>-346.0470726979044</v>
+        <v>0</v>
       </c>
       <c r="X9" t="n">
-        <v>-302.770231542496</v>
+        <v>0</v>
       </c>
       <c r="Y9" t="n">
-        <v>-283.0975195669943</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -8782,76 +8782,76 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-330.8657055718805</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>-312.5986355576808</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>-302.5194122782605</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>-287.6344989330975</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>-285.9374865868901</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>-293.0534320728443</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>-297.2998549933121</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>-280.566</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>-289.718</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>-333.19</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>-333.762</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>-319.748</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>-320.3200000000001</v>
+        <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>-315.172</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>-292.864</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>-293.436</v>
+        <v>0</v>
       </c>
       <c r="R10" t="n">
-        <v>-285.428</v>
+        <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>-307.9904506607303</v>
+        <v>0</v>
       </c>
       <c r="T10" t="n">
-        <v>-354.873879232159</v>
+        <v>0</v>
       </c>
       <c r="U10" t="n">
-        <v>-369.6570220893018</v>
+        <v>0</v>
       </c>
       <c r="V10" t="n">
-        <v>-374.4435484968433</v>
+        <v>0</v>
       </c>
       <c r="W10" t="n">
-        <v>-368.5746222916773</v>
+        <v>0</v>
       </c>
       <c r="X10" t="n">
-        <v>-332.7400610900855</v>
+        <v>0</v>
       </c>
       <c r="Y10" t="n">
-        <v>-331.1336776624333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -11798,76 +11798,76 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-370.4143528989813</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>-349.8745169153619</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-323.2990290295856</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-306.4445982054113</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>-304.2291681757649</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>-318.074690831447</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>-337.378924150804</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>-220.5297692295177</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>-61.78612988525541</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>42.26331273769551</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>149.0026897868758</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>186.498881402574</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>230.6121581694991</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>250.8792143770397</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>221.7830832294987</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>127.75259142622</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>-46.62762742612631</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>-223.6241502545917</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>-391.5955291070197</v>
+        <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>-444.3122552611476</v>
+        <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>-436.0135784144501</v>
+        <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>-425.3355231041314</v>
+        <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>-374.0444019949066</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>-335.7333614715552</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -11877,76 +11877,76 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-288.5780292354309</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>-269.4605762365213</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>-251.562220653923</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>-236.2645485692544</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>-234.8803273813275</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>-245.8072043092885</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>-273.42333901413</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>-157.0476552866256</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>5.939760881895324</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>103.6589765681699</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>198.3703491171894</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>241.036685683637</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>257.0401713830751</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>243.7734863720914</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>184.4628981367973</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>60.16760401915019</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>-107.727892742285</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>-217.7131985152447</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>-326.4262376682347</v>
+        <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>-356.0438733264622</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>-353.8915634556467</v>
+        <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>-346.0470726979044</v>
+        <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>-302.770231542496</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="n">
-        <v>-283.0975195669943</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -11956,76 +11956,76 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-330.8657055718805</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>-312.5986355576808</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>-302.5194122782605</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>-287.6344989330975</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>-285.9374865868901</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>-293.0534320728443</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>-297.2998549933121</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>-164.1055743142987</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>-25.7973078035875</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>46.64212076784105</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>121.2158350535553</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>165.9584064821267</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>145.3549779106981</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>89.60297791069814</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>16.51954933926959</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>-117.0038792321589</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>-251.3930220893018</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>-307.9904506607303</v>
+        <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>-354.873879232159</v>
+        <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>-369.6570220893018</v>
+        <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>-374.4435484968433</v>
+        <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>-368.5746222916773</v>
+        <v>0</v>
       </c>
       <c r="X4" t="n">
-        <v>-332.7400610900855</v>
+        <v>0</v>
       </c>
       <c r="Y4" t="n">
-        <v>-331.1336776624333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -12035,76 +12035,76 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-370.4143528989813</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>-349.8745169153619</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>-323.2990290295856</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>-306.4445982054113</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>-304.2291681757649</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>-318.074690831447</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>-337.378924150804</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>-220.5297692295177</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>-61.78612988525541</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>42.26331273769551</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>149.0026897868758</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>186.498881402574</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>230.6121581694991</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>250.8792143770397</v>
+        <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>221.7830832294987</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>127.75259142622</v>
+        <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>-46.62762742612631</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>-223.6241502545917</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>-391.5955291070197</v>
+        <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>-444.3122552611476</v>
+        <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>-436.0135784144501</v>
+        <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>-425.3355231041314</v>
+        <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>-374.0444019949066</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="n">
-        <v>-335.7333614715552</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -12114,76 +12114,76 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-288.5780292354309</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>-269.4605762365213</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>-251.562220653923</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>-236.2645485692544</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>-234.8803273813275</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>-245.8072043092885</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>-273.42333901413</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>-157.0476552866256</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>5.939760881895324</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>103.6589765681699</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>198.3703491171894</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>241.036685683637</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>257.0401713830751</v>
+        <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>243.7734863720914</v>
+        <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>184.4628981367973</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>60.16760401915019</v>
+        <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>-107.727892742285</v>
+        <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>-217.7131985152447</v>
+        <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>-326.4262376682347</v>
+        <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>-356.0438733264622</v>
+        <v>0</v>
       </c>
       <c r="V6" t="n">
-        <v>-353.8915634556467</v>
+        <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>-346.0470726979044</v>
+        <v>0</v>
       </c>
       <c r="X6" t="n">
-        <v>-302.770231542496</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="n">
-        <v>-283.0975195669943</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -12193,76 +12193,76 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-330.8657055718805</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>-312.5986355576808</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>-302.5194122782605</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>-287.6344989330975</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>-285.9374865868901</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>-293.0534320728443</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>-297.2998549933121</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>-164.1055743142987</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>-25.7973078035875</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>46.64212076784105</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>121.2158350535553</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>165.9584064821267</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>145.3549779106981</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>89.60297791069814</v>
+        <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>16.51954933926959</v>
+        <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>-117.0038792321589</v>
+        <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>-251.3930220893018</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>-307.9904506607303</v>
+        <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>-354.873879232159</v>
+        <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>-369.6570220893018</v>
+        <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>-374.4435484968433</v>
+        <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>-368.5746222916773</v>
+        <v>0</v>
       </c>
       <c r="X7" t="n">
-        <v>-332.7400610900855</v>
+        <v>0</v>
       </c>
       <c r="Y7" t="n">
-        <v>-331.1336776624333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -12272,76 +12272,76 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-370.4143528989813</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>-349.8745169153619</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>-323.2990290295856</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>-306.4445982054113</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>-304.2291681757649</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>-318.074690831447</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>-337.378924150804</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>-220.5297692295177</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>-61.78612988525541</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>42.26331273769551</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>149.0026897868758</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>186.498881402574</v>
+        <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>230.6121581694991</v>
+        <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>250.8792143770397</v>
+        <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>221.7830832294987</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>127.75259142622</v>
+        <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>-46.62762742612631</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>-223.6241502545917</v>
+        <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>-391.5955291070197</v>
+        <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>-444.3122552611476</v>
+        <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>-436.0135784144501</v>
+        <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>-425.3355231041314</v>
+        <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>-374.0444019949066</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="n">
-        <v>-335.7333614715552</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -12351,76 +12351,76 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-288.5780292354309</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>-269.4605762365213</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>-251.562220653923</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>-236.2645485692544</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>-234.8803273813275</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>-245.8072043092885</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>-273.42333901413</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>-157.0476552866256</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>5.939760881895324</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>103.6589765681699</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>198.3703491171894</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>241.036685683637</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>257.0401713830751</v>
+        <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>243.7734863720914</v>
+        <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>184.4628981367973</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>60.16760401915019</v>
+        <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>-107.727892742285</v>
+        <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>-217.7131985152447</v>
+        <v>0</v>
       </c>
       <c r="T9" t="n">
-        <v>-326.4262376682347</v>
+        <v>0</v>
       </c>
       <c r="U9" t="n">
-        <v>-356.0438733264622</v>
+        <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>-353.8915634556467</v>
+        <v>0</v>
       </c>
       <c r="W9" t="n">
-        <v>-346.0470726979044</v>
+        <v>0</v>
       </c>
       <c r="X9" t="n">
-        <v>-302.770231542496</v>
+        <v>0</v>
       </c>
       <c r="Y9" t="n">
-        <v>-283.0975195669943</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -12430,76 +12430,76 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-330.8657055718805</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>-312.5986355576808</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>-302.5194122782605</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>-287.6344989330975</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>-285.9374865868901</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>-293.0534320728443</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>-297.2998549933121</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>-164.1055743142987</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>-25.7973078035875</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>46.64212076784105</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>121.2158350535553</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>165.9584064821267</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>145.3549779106981</v>
+        <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>89.60297791069814</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>16.51954933926959</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>-117.0038792321589</v>
+        <v>0</v>
       </c>
       <c r="R10" t="n">
-        <v>-251.3930220893018</v>
+        <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>-307.9904506607303</v>
+        <v>0</v>
       </c>
       <c r="T10" t="n">
-        <v>-354.873879232159</v>
+        <v>0</v>
       </c>
       <c r="U10" t="n">
-        <v>-369.6570220893018</v>
+        <v>0</v>
       </c>
       <c r="V10" t="n">
-        <v>-374.4435484968433</v>
+        <v>0</v>
       </c>
       <c r="W10" t="n">
-        <v>-368.5746222916773</v>
+        <v>0</v>
       </c>
       <c r="X10" t="n">
-        <v>-332.7400610900855</v>
+        <v>0</v>
       </c>
       <c r="Y10" t="n">
-        <v>-331.1336776624333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -15467,37 +15467,37 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>56.31823077048233</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>221.6398701147446</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>366.8733127376955</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>471.6106897868758</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>493.090881402574</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>535.4881581694991</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>548.3192143770397</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>494.6270832294987</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>399.16659142622</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>214.7763725738737</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>30.62984974540833</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
         <v>0</v>
@@ -15546,34 +15546,34 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>63.17234471337443</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>234.7397608818953</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>375.3589765681699</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>470.0703491171894</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>498.436685683637</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>514.4401713830752</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>495.4534863720914</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>413.2628981367973</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>288.9676040191502</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>112.492107257715</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -15625,34 +15625,34 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>116.4604256857013</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>263.9206921964125</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>379.832120767841</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>454.9778350535553</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>485.7064064821268</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>465.6749779106981</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>404.7749779106982</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>309.3835493392696</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>176.432120767841</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>34.0349779106982</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
@@ -15704,37 +15704,37 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>56.31823077048233</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>221.6398701147446</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>366.8733127376955</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>471.6106897868758</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>493.090881402574</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>535.4881581694991</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>548.3192143770397</v>
+        <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>494.6270832294987</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>399.16659142622</v>
+        <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>214.7763725738737</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>30.62984974540833</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
         <v>0</v>
@@ -15783,34 +15783,34 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>63.17234471337443</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>234.7397608818953</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>375.3589765681699</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>470.0703491171894</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>498.436685683637</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>514.4401713830752</v>
+        <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>495.4534863720914</v>
+        <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>413.2628981367973</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>288.9676040191502</v>
+        <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>112.492107257715</v>
+        <v>0</v>
       </c>
       <c r="S6" t="n">
         <v>0</v>
@@ -15862,34 +15862,34 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>116.4604256857013</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>263.9206921964125</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>379.832120767841</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>454.9778350535553</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>485.7064064821268</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>465.6749779106981</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>404.7749779106982</v>
+        <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>309.3835493392696</v>
+        <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>176.432120767841</v>
+        <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>34.0349779106982</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
         <v>0</v>
@@ -15941,37 +15941,37 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>56.31823077048233</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>221.6398701147446</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>366.8733127376955</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>471.6106897868758</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>493.090881402574</v>
+        <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>535.4881581694991</v>
+        <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>548.3192143770397</v>
+        <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>494.6270832294987</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>399.16659142622</v>
+        <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>214.7763725738737</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>30.62984974540833</v>
+        <v>0</v>
       </c>
       <c r="T8" t="n">
         <v>0</v>
@@ -16020,34 +16020,34 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>63.17234471337443</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>234.7397608818953</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>375.3589765681699</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>470.0703491171894</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>498.436685683637</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>514.4401713830752</v>
+        <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>495.4534863720914</v>
+        <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>413.2628981367973</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>288.9676040191502</v>
+        <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>112.492107257715</v>
+        <v>0</v>
       </c>
       <c r="S9" t="n">
         <v>0</v>
@@ -16099,34 +16099,34 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>116.4604256857013</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>263.9206921964125</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>379.832120767841</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>454.9778350535553</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>485.7064064821268</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>465.6749779106981</v>
+        <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>404.7749779106982</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>309.3835493392696</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>176.432120767841</v>
+        <v>0</v>
       </c>
       <c r="R10" t="n">
-        <v>34.0349779106982</v>
+        <v>0</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -19094,31 +19094,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>37.04143528989812</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>34.98745169153618</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>32.32990290295855</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>30.64445982054112</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>30.42291681757649</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>31.80746908314469</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>33.73789241508039</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>27.68479999999999</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>28.3426</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -19142,28 +19142,28 @@
         <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>26.1404</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>25.42539999999999</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>39.15955291070196</v>
+        <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>44.43122552611475</v>
+        <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>43.601357841445</v>
+        <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>42.53355231041314</v>
+        <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>37.40444019949065</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>33.57333614715552</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -19173,28 +19173,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>28.85780292354308</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>26.94605762365213</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>25.1562220653923</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>23.62645485692543</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>23.48803273813274</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>24.58072043092885</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>27.34233390141299</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>22.02199999999999</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -19221,28 +19221,28 @@
         <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>22.02199999999999</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>21.77131985152446</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>32.64262376682346</v>
+        <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>35.60438733264621</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>35.38915634556466</v>
+        <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>34.60470726979043</v>
+        <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>30.2770231542496</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="n">
-        <v>28.30975195669942</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -19252,31 +19252,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>33.08657055718805</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>31.25986355576808</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>30.25194122782604</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>28.76344989330974</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>28.593748658689</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>29.30534320728443</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>29.72998549933121</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>28.05659999999999</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>25.7973078035875</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -19297,31 +19297,31 @@
         <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>29.3436</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>28.54279999999999</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>30.79904506607303</v>
+        <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>35.48738792321589</v>
+        <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>36.96570220893017</v>
+        <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>37.44435484968432</v>
+        <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>36.85746222916772</v>
+        <v>0</v>
       </c>
       <c r="X4" t="n">
-        <v>33.27400610900855</v>
+        <v>0</v>
       </c>
       <c r="Y4" t="n">
-        <v>33.11336776624331</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -19331,31 +19331,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>37.04143528989812</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>34.98745169153617</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>32.32990290295854</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>30.64445982054112</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>30.42291681757647</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>31.80746908314469</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>33.73789241508038</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>27.68479999999999</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>28.3426</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
@@ -19379,28 +19379,28 @@
         <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>26.1404</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>25.42539999999999</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>39.15955291070195</v>
+        <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>44.43122552611474</v>
+        <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>43.60135784144499</v>
+        <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>42.53355231041312</v>
+        <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>37.40444019949065</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="n">
-        <v>33.57333614715552</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -19410,28 +19410,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>28.85780292354308</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>26.94605762365213</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>25.15622206539229</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>23.62645485692543</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>23.48803273813274</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>24.58072043092885</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>27.34233390141299</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>22.02199999999999</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -19458,28 +19458,28 @@
         <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>22.02199999999999</v>
+        <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>21.77131985152447</v>
+        <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>32.64262376682346</v>
+        <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>35.60438733264621</v>
+        <v>0</v>
       </c>
       <c r="V6" t="n">
-        <v>35.38915634556466</v>
+        <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>34.60470726979043</v>
+        <v>0</v>
       </c>
       <c r="X6" t="n">
-        <v>30.27702315424959</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="n">
-        <v>28.30975195669942</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -19489,31 +19489,31 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>33.08657055718805</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>31.25986355576808</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>30.25194122782604</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>28.76344989330974</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>28.593748658689</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>29.30534320728442</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>29.72998549933121</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>28.05659999999999</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>25.79730780358756</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
@@ -19534,31 +19534,31 @@
         <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>29.3436</v>
+        <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>28.54279999999999</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>30.79904506607303</v>
+        <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>35.48738792321588</v>
+        <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>36.96570220893016</v>
+        <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>37.44435484968432</v>
+        <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>36.85746222916771</v>
+        <v>0</v>
       </c>
       <c r="X7" t="n">
-        <v>33.27400610900855</v>
+        <v>0</v>
       </c>
       <c r="Y7" t="n">
-        <v>33.11336776624331</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -19568,31 +19568,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>37.04143528989812</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>34.98745169153618</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>32.32990290295855</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>30.64445982054112</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>30.42291681757649</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>31.80746908314469</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>33.73789241508039</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>27.68479999999999</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>28.3426</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
@@ -19616,28 +19616,28 @@
         <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>26.1404</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>25.42539999999999</v>
+        <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>39.15955291070197</v>
+        <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>44.43122552611476</v>
+        <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>43.60135784144499</v>
+        <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>42.53355231041313</v>
+        <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>37.40444019949065</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="n">
-        <v>33.57333614715552</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -19647,28 +19647,28 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>28.85780292354308</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>26.94605762365213</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>25.1562220653923</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>23.62645485692543</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>23.48803273813274</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>24.58072043092885</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>27.34233390141299</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>22.02199999999999</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -19695,28 +19695,28 @@
         <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>22.02199999999999</v>
+        <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>21.77131985152447</v>
+        <v>0</v>
       </c>
       <c r="T9" t="n">
-        <v>32.64262376682346</v>
+        <v>0</v>
       </c>
       <c r="U9" t="n">
-        <v>35.60438733264622</v>
+        <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>35.38915634556466</v>
+        <v>0</v>
       </c>
       <c r="W9" t="n">
-        <v>34.60470726979042</v>
+        <v>0</v>
       </c>
       <c r="X9" t="n">
-        <v>30.2770231542496</v>
+        <v>0</v>
       </c>
       <c r="Y9" t="n">
-        <v>28.30975195669942</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -19726,31 +19726,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>33.08657055718805</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>31.25986355576808</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>30.25194122782604</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>28.76344989330974</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>28.593748658689</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>29.30534320728443</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>29.72998549933121</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>28.05659999999999</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>25.7973078035875</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
@@ -19771,31 +19771,31 @@
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>29.3436</v>
+        <v>0</v>
       </c>
       <c r="R10" t="n">
-        <v>28.5428</v>
+        <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>30.79904506607303</v>
+        <v>0</v>
       </c>
       <c r="T10" t="n">
-        <v>35.48738792321588</v>
+        <v>0</v>
       </c>
       <c r="U10" t="n">
-        <v>36.96570220893017</v>
+        <v>0</v>
       </c>
       <c r="V10" t="n">
-        <v>37.44435484968432</v>
+        <v>0</v>
       </c>
       <c r="W10" t="n">
-        <v>36.85746222916771</v>
+        <v>0</v>
       </c>
       <c r="X10" t="n">
-        <v>33.27400610900855</v>
+        <v>0</v>
       </c>
       <c r="Y10" t="n">
-        <v>33.11336776624331</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -22715,13 +22715,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>286</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>286</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>286</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -22767,13 +22767,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -23578,31 +23578,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>333.3729176090832</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>314.8870652238257</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>290.969126126627</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>275.8001383848702</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>273.8062513581884</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>286.2672217483023</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>303.6410317357236</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>192.8449692295177</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>33.44352988525541</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -23626,28 +23626,28 @@
         <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>20.48722742612631</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>198.1987502545917</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>352.4359761963177</v>
+        <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>399.8810297350328</v>
+        <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>392.4122205730051</v>
+        <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>382.8019707937183</v>
+        <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>336.639961795416</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>302.1600253243997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -23657,28 +23657,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>259.7202263118878</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>242.5145186128692</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>226.4059985885307</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>212.638093712329</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>211.3922946431947</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>221.2264838783597</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>246.081005112717</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>135.0256552866256</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -23705,28 +23705,28 @@
         <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>85.70589274228499</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>195.9418786637202</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>293.7836139014112</v>
+        <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>320.439485993816</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>318.5024071100821</v>
+        <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>311.4423654281139</v>
+        <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>272.4932083882464</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="n">
-        <v>254.7877676102948</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -23736,28 +23736,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>297.7791350146925</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>281.3387720019127</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>272.2674710504344</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>258.8710490397877</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>257.3437379282011</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>263.7480888655599</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>267.5698694939809</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>136.0489743142987</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -23781,31 +23781,31 @@
         <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>87.66027923215893</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>222.8502220893018</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>277.1914055946573</v>
+        <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>319.3864913089431</v>
+        <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>332.6913198803716</v>
+        <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>336.999193647159</v>
+        <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>331.7171600625095</v>
+        <v>0</v>
       </c>
       <c r="X4" t="n">
-        <v>299.466054981077</v>
+        <v>0</v>
       </c>
       <c r="Y4" t="n">
-        <v>298.02030989619</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -23815,31 +23815,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>333.3729176090832</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>314.8870652238256</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>290.969126126627</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>275.8001383848702</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>273.8062513581883</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>286.2672217483023</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>303.6410317357236</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>192.8449692295177</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>33.44352988525542</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
@@ -23863,28 +23863,28 @@
         <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>20.48722742612633</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>198.1987502545917</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>352.4359761963177</v>
+        <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>399.8810297350328</v>
+        <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>392.412220573005</v>
+        <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>382.8019707937182</v>
+        <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>336.639961795416</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="n">
-        <v>302.1600253243997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -23894,28 +23894,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>259.7202263118878</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>242.5145186128692</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>226.4059985885307</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>212.638093712329</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>211.3922946431947</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>221.2264838783597</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>246.081005112717</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>135.0256552866256</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -23942,28 +23942,28 @@
         <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>85.70589274228499</v>
+        <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>195.9418786637202</v>
+        <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>293.7836139014112</v>
+        <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>320.439485993816</v>
+        <v>0</v>
       </c>
       <c r="V6" t="n">
-        <v>318.502407110082</v>
+        <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>311.4423654281139</v>
+        <v>0</v>
       </c>
       <c r="X6" t="n">
-        <v>272.4932083882464</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="n">
-        <v>254.7877676102948</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -23973,28 +23973,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>297.7791350146924</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>281.3387720019127</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>272.2674710504344</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>258.8710490397877</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>257.3437379282011</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>263.7480888655599</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>267.5698694939809</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>136.0489743142987</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -24018,31 +24018,31 @@
         <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>87.66027923215898</v>
+        <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>222.8502220893018</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>277.1914055946573</v>
+        <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>319.3864913089431</v>
+        <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>332.6913198803716</v>
+        <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>336.9991936471589</v>
+        <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>331.7171600625095</v>
+        <v>0</v>
       </c>
       <c r="X7" t="n">
-        <v>299.466054981077</v>
+        <v>0</v>
       </c>
       <c r="Y7" t="n">
-        <v>298.0203098961899</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -24052,31 +24052,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>333.3729176090832</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>314.8870652238257</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>290.969126126627</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>275.8001383848701</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>273.8062513581884</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>286.2672217483023</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>303.6410317357236</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>192.8449692295177</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>33.4435298852554</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
@@ -24100,28 +24100,28 @@
         <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>20.48722742612631</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>198.1987502545917</v>
+        <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>352.4359761963177</v>
+        <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>399.8810297350328</v>
+        <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>392.4122205730051</v>
+        <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>382.8019707937183</v>
+        <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>336.6399617954159</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="n">
-        <v>302.1600253243997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -24131,28 +24131,28 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>259.7202263118878</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>242.5145186128692</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>226.4059985885307</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>212.638093712329</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>211.3922946431947</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>221.2264838783597</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>246.081005112717</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>135.0256552866256</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -24179,28 +24179,28 @@
         <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>85.70589274228499</v>
+        <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>195.9418786637202</v>
+        <v>0</v>
       </c>
       <c r="T9" t="n">
-        <v>293.7836139014112</v>
+        <v>0</v>
       </c>
       <c r="U9" t="n">
-        <v>320.439485993816</v>
+        <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>318.5024071100821</v>
+        <v>0</v>
       </c>
       <c r="W9" t="n">
-        <v>311.4423654281139</v>
+        <v>0</v>
       </c>
       <c r="X9" t="n">
-        <v>272.4932083882464</v>
+        <v>0</v>
       </c>
       <c r="Y9" t="n">
-        <v>254.7877676102948</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -24210,28 +24210,28 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>297.7791350146925</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>281.3387720019128</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>272.2674710504344</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>258.8710490397877</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>257.3437379282011</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>263.7480888655599</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>267.5698694939809</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>136.0489743142987</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
@@ -24255,31 +24255,31 @@
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>87.66027923215893</v>
+        <v>0</v>
       </c>
       <c r="R10" t="n">
-        <v>222.8502220893018</v>
+        <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>277.1914055946573</v>
+        <v>0</v>
       </c>
       <c r="T10" t="n">
-        <v>319.3864913089431</v>
+        <v>0</v>
       </c>
       <c r="U10" t="n">
-        <v>332.6913198803716</v>
+        <v>0</v>
       </c>
       <c r="V10" t="n">
-        <v>336.999193647159</v>
+        <v>0</v>
       </c>
       <c r="W10" t="n">
-        <v>331.7171600625095</v>
+        <v>0</v>
       </c>
       <c r="X10" t="n">
-        <v>299.466054981077</v>
+        <v>0</v>
       </c>
       <c r="Y10" t="n">
-        <v>298.0203098961899</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">

</xml_diff>